<commit_message>
Senato fino a art. 17 comma 1 lett. b
</commit_message>
<xml_diff>
--- a/dati_2018/dati_2018.xlsx
+++ b/dati_2018/dati_2018.xlsx
@@ -1,27 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\R\elezioni\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\R\elezioni\dati_2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2292BBBF-349B-4514-AC22-5FA094D291E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9701B99-7311-4275-9527-B982BBF36831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="camera_liste" sheetId="2" r:id="rId1"/>
-    <sheet name="camera_pluri" sheetId="1" r:id="rId2"/>
+    <sheet name="senato_liste" sheetId="3" r:id="rId2"/>
+    <sheet name="camera_pluri" sheetId="1" r:id="rId3"/>
+    <sheet name="senato_pluri" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="158">
   <si>
     <t>CIRCOSCRIZIONE</t>
   </si>
@@ -414,6 +428,87 @@
   </si>
   <si>
     <t>MINORANZA</t>
+  </si>
+  <si>
+    <t>DEMOCRAZIA CRISTIANA</t>
+  </si>
+  <si>
+    <t>DESTRE UNITE - FORCONI</t>
+  </si>
+  <si>
+    <t>SMS - STATO MODERNO SOLIDALE</t>
+  </si>
+  <si>
+    <t>PIEMONTE</t>
+  </si>
+  <si>
+    <t>PIEMONTE - 01</t>
+  </si>
+  <si>
+    <t>PIEMONTE - 02</t>
+  </si>
+  <si>
+    <t>LOMBARDIA</t>
+  </si>
+  <si>
+    <t>LOMBARDIA - 01</t>
+  </si>
+  <si>
+    <t>LOMBARDIA - 02</t>
+  </si>
+  <si>
+    <t>LOMBARDIA - 03</t>
+  </si>
+  <si>
+    <t>LOMBARDIA - 04</t>
+  </si>
+  <si>
+    <t>LOMBARDIA - 05</t>
+  </si>
+  <si>
+    <t>TRENTINO-ALTO ADIGE</t>
+  </si>
+  <si>
+    <t>VENETO</t>
+  </si>
+  <si>
+    <t>VENETO - 01</t>
+  </si>
+  <si>
+    <t>VENETO - 02</t>
+  </si>
+  <si>
+    <t>LAZIO</t>
+  </si>
+  <si>
+    <t>LAZIO - 01</t>
+  </si>
+  <si>
+    <t>LAZIO - 02</t>
+  </si>
+  <si>
+    <t>LAZIO - 03</t>
+  </si>
+  <si>
+    <t>CAMPANIA</t>
+  </si>
+  <si>
+    <t>CAMPANIA - 01</t>
+  </si>
+  <si>
+    <t>CAMPANIA - 02</t>
+  </si>
+  <si>
+    <t>CAMPANIA - 03</t>
+  </si>
+  <si>
+    <t>SICILIA</t>
+  </si>
+  <si>
+    <t>SICILIA - 01</t>
+  </si>
+  <si>
+    <t>SICILIA - 02</t>
   </si>
 </sst>
 </file>
@@ -1257,8 +1352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF070AD3-6E98-4319-9AB9-7C71230D3C20}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1568,11 +1663,325 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00CBD48A-5BFE-4C86-BBDD-7430FC54F38F}">
+  <dimension ref="A1:C33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>115</v>
+      </c>
+      <c r="B14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>109</v>
+      </c>
+      <c r="B19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>103</v>
+      </c>
+      <c r="C24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>99</v>
+      </c>
+      <c r="C28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>133</v>
+      </c>
+      <c r="C32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2293,4 +2702,403 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9936C4CE-A49D-45D8-9361-B5EEEB9DEBBD}">
+  <dimension ref="A1:C35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>144</v>
+      </c>
+      <c r="B10" t="s">
+        <v>145</v>
+      </c>
+      <c r="C10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B20" t="s">
+        <v>148</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>147</v>
+      </c>
+      <c r="B21" t="s">
+        <v>149</v>
+      </c>
+      <c r="C21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>147</v>
+      </c>
+      <c r="B22" t="s">
+        <v>150</v>
+      </c>
+      <c r="C22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>151</v>
+      </c>
+      <c r="B25" t="s">
+        <v>152</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>151</v>
+      </c>
+      <c r="B26" t="s">
+        <v>153</v>
+      </c>
+      <c r="C26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>151</v>
+      </c>
+      <c r="B27" t="s">
+        <v>154</v>
+      </c>
+      <c r="C27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>155</v>
+      </c>
+      <c r="B32" t="s">
+        <v>156</v>
+      </c>
+      <c r="C32">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>155</v>
+      </c>
+      <c r="B33" t="s">
+        <v>157</v>
+      </c>
+      <c r="C33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>